<commit_message>
维保人åMaintenanceWorker data import research realize
</commit_message>
<xml_diff>
--- a/data/database/Synthesis/维保人员数据.xlsx
+++ b/data/database/Synthesis/维保人员数据.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24930" windowHeight="10610" firstSheet="2" activeTab="10"/>
+    <workbookView windowWidth="24930" windowHeight="10610" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="维保人员" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1245" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1250" uniqueCount="389">
   <si>
     <t>人员类别</t>
   </si>
@@ -762,6 +762,9 @@
   </si>
   <si>
     <t>正常</t>
+  </si>
+  <si>
+    <t>m0002</t>
   </si>
   <si>
     <t>轮胎车轴故障</t>
@@ -1876,9 +1879,6 @@
   </si>
   <si>
     <t>轮胎车轴维修</t>
-  </si>
-  <si>
-    <t>m0002</t>
   </si>
   <si>
     <t>车门维修</t>
@@ -2947,7 +2947,7 @@
   <dimension ref="A1:L101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L30"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -4403,13 +4403,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B1" t="s">
         <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D1" t="s">
         <v>11</v>
@@ -4437,7 +4437,7 @@
         <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D3" t="s">
         <v>23</v>
@@ -4451,7 +4451,7 @@
         <v>48</v>
       </c>
       <c r="C4" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D4" t="s">
         <v>26</v>
@@ -4465,7 +4465,7 @@
         <v>62</v>
       </c>
       <c r="C5" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="D5" t="s">
         <v>29</v>
@@ -4479,7 +4479,7 @@
         <v>72</v>
       </c>
       <c r="C6" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D6" t="s">
         <v>32</v>
@@ -4493,7 +4493,7 @@
         <v>86</v>
       </c>
       <c r="C7" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -4504,92 +4504,92 @@
         <v>92</v>
       </c>
       <c r="C8" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="2" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="2" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="2" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="2" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="2" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="2" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="2" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="2" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="2" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="3" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
@@ -4597,18 +4597,18 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B24" t="s">
         <v>187</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B25" t="s">
         <v>194</v>
@@ -4617,51 +4617,51 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B26" t="s">
         <v>199</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B27" t="s">
         <v>206</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B28" t="s">
         <v>213</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B29" t="s">
         <v>216</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B30" t="s">
         <v>221</v>
@@ -4670,47 +4670,47 @@
     </row>
     <row r="31" spans="4:4">
       <c r="D31" s="4" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="32" spans="4:4">
       <c r="D32" s="4" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="33" spans="4:4">
       <c r="D33" s="2" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D34" s="2"/>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="38" spans="4:4">
@@ -4718,17 +4718,17 @@
     </row>
     <row r="39" spans="4:4">
       <c r="D39" s="4" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="40" spans="4:4">
       <c r="D40" s="4" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="41" spans="4:4">
       <c r="D41" s="2" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="42" spans="4:4">
@@ -4736,17 +4736,17 @@
     </row>
     <row r="43" spans="4:4">
       <c r="D43" s="4" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="44" spans="4:4">
       <c r="D44" s="4" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="45" spans="4:4">
       <c r="D45" s="2" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="46" spans="4:4">
@@ -4754,17 +4754,17 @@
     </row>
     <row r="47" spans="4:4">
       <c r="D47" s="4" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="48" spans="4:4">
       <c r="D48" s="4" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="49" spans="4:4">
       <c r="D49" s="2" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="50" spans="4:4">
@@ -4772,12 +4772,12 @@
     </row>
     <row r="51" spans="4:4">
       <c r="D51" s="4" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="52" spans="4:4">
       <c r="D52" s="4" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
   </sheetData>
@@ -4791,8 +4791,8 @@
   <sheetPr/>
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14" outlineLevelCol="4"/>
@@ -4802,30 +4802,30 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="E1" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
@@ -4836,16 +4836,16 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>366</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="E3" t="s">
         <v>23</v>
@@ -4856,10 +4856,10 @@
         <v>369</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>370</v>
@@ -4873,10 +4873,10 @@
         <v>371</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>372</v>
@@ -4890,10 +4890,10 @@
         <v>373</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>374</v>
@@ -4907,10 +4907,10 @@
         <v>375</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>376</v>
@@ -4924,13 +4924,13 @@
         <v>377</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="E8" t="s">
         <v>23</v>
@@ -4941,13 +4941,13 @@
         <v>378</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="E9" t="s">
         <v>26</v>
@@ -4958,13 +4958,13 @@
         <v>379</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="E10" t="s">
         <v>29</v>
@@ -4975,13 +4975,13 @@
         <v>380</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="E11" t="s">
         <v>32</v>
@@ -4992,13 +4992,13 @@
         <v>381</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="E12" t="s">
         <v>20</v>
@@ -5009,13 +5009,13 @@
         <v>382</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="E13" t="s">
         <v>23</v>
@@ -5026,13 +5026,13 @@
         <v>383</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="E14" t="s">
         <v>26</v>
@@ -5043,13 +5043,13 @@
         <v>384</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="E15" t="s">
         <v>29</v>
@@ -5060,13 +5060,13 @@
         <v>385</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="E16" t="s">
         <v>32</v>
@@ -5077,13 +5077,13 @@
         <v>386</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="E17" t="s">
         <v>20</v>
@@ -5094,13 +5094,13 @@
         <v>387</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E18" t="s">
         <v>23</v>
@@ -5111,13 +5111,13 @@
         <v>388</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E19" t="s">
         <v>26</v>
@@ -5125,13 +5125,13 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>367</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>366</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>13</v>
@@ -5145,10 +5145,10 @@
         <v>369</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>13</v>
@@ -5162,10 +5162,10 @@
         <v>371</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>13</v>
@@ -5179,10 +5179,10 @@
         <v>373</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>13</v>
@@ -5193,16 +5193,16 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="1" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>368</v>
+        <v>240</v>
       </c>
       <c r="E24" t="s">
         <v>20</v>
@@ -8342,10 +8342,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -8414,54 +8414,53 @@
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" t="str">
+      <c r="A3" t="s">
+        <v>240</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>237</v>
+      </c>
+      <c r="D3" t="s">
+        <v>238</v>
+      </c>
+      <c r="E3" s="5">
+        <v>45073.7534722222</v>
+      </c>
+      <c r="F3" s="5">
+        <v>45073.7638888889</v>
+      </c>
+      <c r="G3" s="5">
+        <v>45073.7951388889</v>
+      </c>
+      <c r="I3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="str">
         <f>_xlfn.CONCAT("m",TEXT(VALUE(RIGHT(A2,4))+1,"0000"))</f>
         <v>m0002</v>
       </c>
-      <c r="B3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" t="s">
-        <v>240</v>
-      </c>
-      <c r="D3" t="s">
-        <v>241</v>
-      </c>
-      <c r="E3" s="5">
-        <v>44862.4652777778</v>
-      </c>
-      <c r="F3" s="5">
-        <v>44862.4791666667</v>
-      </c>
-      <c r="G3" s="5">
-        <v>44862.0086805556</v>
-      </c>
-      <c r="I3" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" t="str">
-        <f t="shared" ref="A4:A7" si="0">_xlfn.CONCAT("m",TEXT(VALUE(RIGHT(A3,4))+1,"0000"))</f>
-        <v>m0003</v>
-      </c>
       <c r="B4" t="s">
         <v>36</v>
       </c>
       <c r="C4" t="s">
+        <v>241</v>
+      </c>
+      <c r="D4" t="s">
         <v>242</v>
       </c>
-      <c r="D4" t="s">
-        <v>243</v>
-      </c>
       <c r="E4" s="5">
-        <v>44908.4666666667</v>
+        <v>44862.4652777778</v>
       </c>
       <c r="F4" s="5">
-        <v>44908.4756944444</v>
+        <v>44862.4791666667</v>
       </c>
       <c r="G4" s="5">
-        <v>44908.4979166667</v>
+        <v>44862.0086805556</v>
       </c>
       <c r="I4" t="s">
         <v>239</v>
@@ -8469,26 +8468,26 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="str">
-        <f t="shared" si="0"/>
-        <v>m0004</v>
+        <f t="shared" ref="A5:A8" si="0">_xlfn.CONCAT("m",TEXT(VALUE(RIGHT(A4,4))+1,"0000"))</f>
+        <v>m0003</v>
       </c>
       <c r="B5" t="s">
         <v>36</v>
       </c>
       <c r="C5" t="s">
+        <v>243</v>
+      </c>
+      <c r="D5" t="s">
         <v>244</v>
       </c>
-      <c r="D5" t="s">
-        <v>245</v>
-      </c>
       <c r="E5" s="5">
-        <v>44899.55</v>
+        <v>44908.4666666667</v>
       </c>
       <c r="F5" s="5">
-        <v>44899.5534722222</v>
+        <v>44908.4756944444</v>
       </c>
       <c r="G5" s="5">
-        <v>44899.5604166667</v>
+        <v>44908.4979166667</v>
       </c>
       <c r="I5" t="s">
         <v>239</v>
@@ -8497,78 +8496,79 @@
     <row r="6" spans="1:9">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
-        <v>m0005</v>
+        <v>m0004</v>
       </c>
       <c r="B6" t="s">
         <v>36</v>
       </c>
       <c r="C6" t="s">
+        <v>245</v>
+      </c>
+      <c r="D6" t="s">
         <v>246</v>
       </c>
-      <c r="D6" t="s">
-        <v>247</v>
-      </c>
       <c r="E6" s="5">
-        <v>44622.7104166667</v>
+        <v>44899.55</v>
       </c>
       <c r="F6" s="5">
-        <v>44622.7229166667</v>
+        <v>44899.5534722222</v>
       </c>
       <c r="G6" s="5">
-        <v>44622.7368055556</v>
+        <v>44899.5604166667</v>
       </c>
       <c r="I6" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
-        <v>m0006</v>
+        <v>m0005</v>
       </c>
       <c r="B7" t="s">
         <v>36</v>
       </c>
       <c r="C7" t="s">
+        <v>247</v>
+      </c>
+      <c r="D7" t="s">
+        <v>248</v>
+      </c>
+      <c r="E7" s="5">
+        <v>44622.7104166667</v>
+      </c>
+      <c r="F7" s="5">
+        <v>44622.7229166667</v>
+      </c>
+      <c r="G7" s="5">
+        <v>44622.7368055556</v>
+      </c>
+      <c r="I7" t="s">
         <v>249</v>
       </c>
-      <c r="D7" t="s">
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="str">
+        <f t="shared" si="0"/>
+        <v>m0006</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s">
         <v>250</v>
       </c>
-      <c r="E7" s="5">
+      <c r="D8" t="s">
+        <v>251</v>
+      </c>
+      <c r="E8" s="5">
         <v>44562.4590277778</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F8" s="5">
         <v>44562.4756944444</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G8" s="5">
         <v>44562.4854166667</v>
-      </c>
-      <c r="I7" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" t="s">
-        <v>251</v>
-      </c>
-      <c r="B8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" t="s">
-        <v>252</v>
-      </c>
-      <c r="D8" t="s">
-        <v>253</v>
-      </c>
-      <c r="E8" s="5">
-        <v>44853.8402777778</v>
-      </c>
-      <c r="F8" s="5">
-        <v>44853.8472222222</v>
-      </c>
-      <c r="G8" s="5">
-        <v>44853.8541666667</v>
       </c>
       <c r="I8" t="s">
         <v>239</v>
@@ -8576,25 +8576,25 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B9" t="s">
         <v>48</v>
       </c>
       <c r="C9" t="s">
+        <v>253</v>
+      </c>
+      <c r="D9" t="s">
         <v>254</v>
       </c>
-      <c r="D9" t="s">
-        <v>255</v>
-      </c>
       <c r="E9" s="5">
-        <v>45005.91875</v>
+        <v>44853.8402777778</v>
       </c>
       <c r="F9" s="5">
-        <v>45005.9256944444</v>
+        <v>44853.8472222222</v>
       </c>
       <c r="G9" s="5">
-        <v>45005.9326388889</v>
+        <v>44853.8541666667</v>
       </c>
       <c r="I9" t="s">
         <v>239</v>
@@ -8602,25 +8602,25 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B10" t="s">
         <v>48</v>
       </c>
       <c r="C10" t="s">
+        <v>255</v>
+      </c>
+      <c r="D10" t="s">
         <v>256</v>
       </c>
-      <c r="D10" t="s">
-        <v>257</v>
-      </c>
       <c r="E10" s="5">
-        <v>44707.6701388889</v>
+        <v>45005.91875</v>
       </c>
       <c r="F10" s="5">
-        <v>44707.6770833333</v>
+        <v>45005.9256944444</v>
       </c>
       <c r="G10" s="5">
-        <v>44707.6840277778</v>
+        <v>45005.9326388889</v>
       </c>
       <c r="I10" t="s">
         <v>239</v>
@@ -8628,77 +8628,77 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
+        <v>252</v>
+      </c>
+      <c r="B11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" t="s">
+        <v>257</v>
+      </c>
+      <c r="D11" t="s">
         <v>258</v>
       </c>
-      <c r="B11" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" t="s">
-        <v>259</v>
-      </c>
-      <c r="D11" t="s">
-        <v>260</v>
-      </c>
       <c r="E11" s="5">
-        <v>44815.7145833333</v>
+        <v>44707.6701388889</v>
       </c>
       <c r="F11" s="5">
-        <v>44815.7215277778</v>
+        <v>44707.6770833333</v>
       </c>
       <c r="G11" s="5">
-        <v>44815.7284722222</v>
+        <v>44707.6840277778</v>
       </c>
       <c r="I11" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B12" t="s">
         <v>62</v>
       </c>
       <c r="C12" t="s">
+        <v>260</v>
+      </c>
+      <c r="D12" t="s">
         <v>261</v>
       </c>
-      <c r="D12" t="s">
-        <v>262</v>
-      </c>
       <c r="E12" s="5">
-        <v>44602.7930555556</v>
+        <v>44815.7145833333</v>
       </c>
       <c r="F12" s="5">
-        <v>44602.8</v>
+        <v>44815.7215277778</v>
       </c>
       <c r="G12" s="5">
-        <v>44602.8069444444</v>
+        <v>44815.7284722222</v>
       </c>
       <c r="I12" t="s">
-        <v>239</v>
+        <v>249</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
+        <v>259</v>
+      </c>
+      <c r="B13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" t="s">
+        <v>262</v>
+      </c>
+      <c r="D13" t="s">
         <v>263</v>
       </c>
-      <c r="B13" t="s">
-        <v>72</v>
-      </c>
-      <c r="C13" t="s">
-        <v>264</v>
-      </c>
-      <c r="D13" t="s">
-        <v>265</v>
-      </c>
       <c r="E13" s="5">
-        <v>44728.4208333333</v>
+        <v>44602.7930555556</v>
       </c>
       <c r="F13" s="5">
-        <v>44728.4277777778</v>
+        <v>44602.8</v>
       </c>
       <c r="G13" s="5">
-        <v>44728.4347222222</v>
+        <v>44602.8069444444</v>
       </c>
       <c r="I13" t="s">
         <v>239</v>
@@ -8706,25 +8706,25 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B14" t="s">
         <v>72</v>
       </c>
       <c r="C14" t="s">
+        <v>265</v>
+      </c>
+      <c r="D14" t="s">
         <v>266</v>
       </c>
-      <c r="D14" t="s">
-        <v>267</v>
-      </c>
       <c r="E14" s="5">
-        <v>44626.79375</v>
+        <v>44728.4208333333</v>
       </c>
       <c r="F14" s="5">
-        <v>44626.8006944444</v>
+        <v>44728.4277777778</v>
       </c>
       <c r="G14" s="5">
-        <v>44626.8076388889</v>
+        <v>44728.4347222222</v>
       </c>
       <c r="I14" t="s">
         <v>239</v>
@@ -8732,25 +8732,25 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B15" t="s">
         <v>72</v>
       </c>
       <c r="C15" t="s">
+        <v>267</v>
+      </c>
+      <c r="D15" t="s">
         <v>268</v>
       </c>
-      <c r="D15" t="s">
-        <v>269</v>
-      </c>
       <c r="E15" s="5">
-        <v>44724.0875</v>
+        <v>44626.79375</v>
       </c>
       <c r="F15" s="5">
-        <v>44724.0944444444</v>
+        <v>44626.8006944444</v>
       </c>
       <c r="G15" s="5">
-        <v>44724.1013888889</v>
+        <v>44626.8076388889</v>
       </c>
       <c r="I15" t="s">
         <v>239</v>
@@ -8758,25 +8758,25 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B16" t="s">
         <v>72</v>
       </c>
       <c r="C16" t="s">
+        <v>269</v>
+      </c>
+      <c r="D16" t="s">
         <v>270</v>
       </c>
-      <c r="D16" t="s">
-        <v>271</v>
-      </c>
       <c r="E16" s="5">
-        <v>44583.7090277778</v>
+        <v>44724.0875</v>
       </c>
       <c r="F16" s="5">
-        <v>44583.7159722222</v>
+        <v>44724.0944444444</v>
       </c>
       <c r="G16" s="5">
-        <v>44583.7229166667</v>
+        <v>44724.1013888889</v>
       </c>
       <c r="I16" t="s">
         <v>239</v>
@@ -8784,25 +8784,25 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
+        <v>264</v>
+      </c>
+      <c r="B17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" t="s">
+        <v>271</v>
+      </c>
+      <c r="D17" t="s">
         <v>272</v>
       </c>
-      <c r="B17" t="s">
-        <v>86</v>
-      </c>
-      <c r="C17" t="s">
-        <v>273</v>
-      </c>
-      <c r="D17" t="s">
-        <v>274</v>
-      </c>
       <c r="E17" s="5">
-        <v>44921.425</v>
+        <v>44583.7090277778</v>
       </c>
       <c r="F17" s="5">
-        <v>44921.4319444444</v>
+        <v>44583.7159722222</v>
       </c>
       <c r="G17" s="5">
-        <v>44921.4388888889</v>
+        <v>44583.7229166667</v>
       </c>
       <c r="I17" t="s">
         <v>239</v>
@@ -8810,53 +8810,79 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
+        <v>273</v>
+      </c>
+      <c r="B18" t="s">
+        <v>86</v>
+      </c>
+      <c r="C18" t="s">
+        <v>274</v>
+      </c>
+      <c r="D18" t="s">
         <v>275</v>
       </c>
-      <c r="B18" t="s">
-        <v>92</v>
-      </c>
-      <c r="C18" t="s">
-        <v>276</v>
-      </c>
-      <c r="D18" t="s">
-        <v>277</v>
-      </c>
       <c r="E18" s="5">
-        <v>44733.2125</v>
+        <v>44921.425</v>
       </c>
       <c r="F18" s="5">
-        <v>44733.2194444444</v>
+        <v>44921.4319444444</v>
       </c>
       <c r="G18" s="5">
-        <v>44733.2263888889</v>
+        <v>44921.4388888889</v>
       </c>
       <c r="I18" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B19" t="s">
         <v>92</v>
       </c>
       <c r="C19" t="s">
+        <v>277</v>
+      </c>
+      <c r="D19" t="s">
         <v>278</v>
       </c>
-      <c r="D19" t="s">
-        <v>260</v>
-      </c>
       <c r="E19" s="5">
+        <v>44733.2125</v>
+      </c>
+      <c r="F19" s="5">
+        <v>44733.2194444444</v>
+      </c>
+      <c r="G19" s="5">
+        <v>44733.2263888889</v>
+      </c>
+      <c r="I19" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" t="s">
+        <v>276</v>
+      </c>
+      <c r="B20" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" t="s">
+        <v>279</v>
+      </c>
+      <c r="D20" t="s">
+        <v>261</v>
+      </c>
+      <c r="E20" s="5">
         <v>44805.2145833333</v>
       </c>
-      <c r="F19" s="5">
+      <c r="F20" s="5">
         <v>44805.2215277778</v>
       </c>
-      <c r="G19" s="5">
+      <c r="G20" s="5">
         <v>44805.2284722222</v>
       </c>
-      <c r="I19" t="s">
+      <c r="I20" t="s">
         <v>239</v>
       </c>
     </row>
@@ -8896,19 +8922,19 @@
         <v>228</v>
       </c>
       <c r="D1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="E1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="F1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="G1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="H1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -8922,13 +8948,13 @@
         <v>45146.4166666667</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="E2" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="G2" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -8943,13 +8969,13 @@
         <v>40992.9583333333</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="E3" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="G3" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -8964,13 +8990,13 @@
         <v>41464.9166666667</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="E4" t="s">
+        <v>290</v>
+      </c>
+      <c r="G4" t="s">
         <v>289</v>
-      </c>
-      <c r="G4" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -8985,13 +9011,13 @@
         <v>42386.8333333333</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="E5" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="G5" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -9006,13 +9032,13 @@
         <v>44538.7916666667</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="E6" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="G6" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -9027,13 +9053,13 @@
         <v>43390.8333333333</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="E7" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="G7" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -9048,13 +9074,13 @@
         <v>39119.4166666667</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="E8" t="s">
+        <v>290</v>
+      </c>
+      <c r="G8" t="s">
         <v>289</v>
-      </c>
-      <c r="G8" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -9069,13 +9095,13 @@
         <v>40728.5833333333</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="E9" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="G9" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -9089,13 +9115,13 @@
         <v>37968.7083333333</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="E10" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="G10" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -9110,13 +9136,13 @@
         <v>39338.9166666667</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="E11" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="G11" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -9131,13 +9157,13 @@
         <v>44843.6666666667</v>
       </c>
       <c r="D12" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="E12" t="s">
+        <v>290</v>
+      </c>
+      <c r="G12" t="s">
         <v>292</v>
-      </c>
-      <c r="E12" t="s">
-        <v>289</v>
-      </c>
-      <c r="G12" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -9152,13 +9178,13 @@
         <v>39812.9166666667</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="E13" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="G13" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -9173,13 +9199,13 @@
         <v>38918.7916666667</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="E14" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="G14" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -9194,13 +9220,13 @@
         <v>41359.8333333333</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="E15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="G15" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -9215,13 +9241,13 @@
         <v>37716.7916666667</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="E16" t="s">
+        <v>290</v>
+      </c>
+      <c r="G16" t="s">
         <v>289</v>
-      </c>
-      <c r="G16" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -9236,13 +9262,13 @@
         <v>41625.9166666667</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="E17" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="G17" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
   </sheetData>
@@ -9276,25 +9302,25 @@
         <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="E1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="F1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="G1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="H1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="I1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -9305,7 +9331,7 @@
         <v>187</v>
       </c>
       <c r="C2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D2" s="5">
         <v>44835.4166666667</v>
@@ -9314,21 +9340,21 @@
         <v>44835.5</v>
       </c>
       <c r="G2" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="H2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B3" t="s">
         <v>194</v>
       </c>
       <c r="C3" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D3" s="5">
         <v>44909.3333333333</v>
@@ -9337,21 +9363,21 @@
         <v>44909.75</v>
       </c>
       <c r="G3" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="H3" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B4" t="s">
         <v>199</v>
       </c>
       <c r="C4" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D4" s="5">
         <v>44873.7083333333</v>
@@ -9360,21 +9386,21 @@
         <v>44873.9166666667</v>
       </c>
       <c r="G4" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="H4" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B5" t="s">
         <v>206</v>
       </c>
       <c r="C5" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D5" s="5">
         <v>44851.8333333333</v>
@@ -9383,21 +9409,21 @@
         <v>44852</v>
       </c>
       <c r="G5" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="H5" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B6" t="s">
         <v>213</v>
       </c>
       <c r="C6" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D6" s="5">
         <v>44658.2083333333</v>
@@ -9406,21 +9432,21 @@
         <v>44658.5</v>
       </c>
       <c r="G6" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="H6" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B7" t="s">
         <v>216</v>
       </c>
       <c r="C7" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D7" s="5">
         <v>44897.5416666667</v>
@@ -9429,21 +9455,21 @@
         <v>44897.75</v>
       </c>
       <c r="G7" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="H7" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B8" t="s">
         <v>221</v>
       </c>
       <c r="C8" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D8" s="5">
         <v>44646.3333333333</v>
@@ -9452,10 +9478,10 @@
         <v>44646.5</v>
       </c>
       <c r="G8" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="H8" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -9466,7 +9492,7 @@
         <v>187</v>
       </c>
       <c r="C9" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D9" s="5">
         <v>44691.6666666667</v>
@@ -9475,21 +9501,21 @@
         <v>44691.9166666667</v>
       </c>
       <c r="G9" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="H9" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B10" t="s">
         <v>194</v>
       </c>
       <c r="C10" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D10" s="5">
         <v>44838.25</v>
@@ -9498,21 +9524,21 @@
         <v>44838.4166666667</v>
       </c>
       <c r="G10" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="H10" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B11" t="s">
         <v>199</v>
       </c>
       <c r="C11" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D11" s="5">
         <v>45104.3333333333</v>
@@ -9521,21 +9547,21 @@
         <v>45104.5</v>
       </c>
       <c r="G11" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="H11" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B12" t="s">
         <v>206</v>
       </c>
       <c r="C12" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D12" s="5">
         <v>44667.5416666667</v>
@@ -9544,24 +9570,24 @@
         <v>44667.7916666667</v>
       </c>
       <c r="G12" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="H12" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="N12" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B13" t="s">
         <v>213</v>
       </c>
       <c r="C13" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D13" s="5">
         <v>44906.7083333333</v>
@@ -9570,21 +9596,21 @@
         <v>44906.9166666667</v>
       </c>
       <c r="G13" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="H13" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B14" t="s">
         <v>216</v>
       </c>
       <c r="C14" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D14" s="5">
         <v>44823.625</v>
@@ -9593,21 +9619,21 @@
         <v>44823.875</v>
       </c>
       <c r="G14" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="H14" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B15" t="s">
         <v>221</v>
       </c>
       <c r="C15" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D15" s="5">
         <v>45098.6666666667</v>
@@ -9616,10 +9642,10 @@
         <v>45098.9583333333</v>
       </c>
       <c r="G15" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="H15" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="16" spans="4:4">

</xml_diff>